<commit_message>
CharData, SkillData 코드명 수정
</commit_message>
<xml_diff>
--- a/Defence2D/Game_Design/DataTable/CharData.xlsx
+++ b/Defence2D/Game_Design/DataTable/CharData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SIDE_PROJECT\Defence2D\Game_Design\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5391F884-CD58-43F2-899A-2B8772C63373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53344DBB-B444-4CFA-A8F2-37E21A5A7E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,10 +1040,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>ChaArcher001</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>궁수</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1056,10 +1052,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>ChaKnight001</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Knight001</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1100,10 +1092,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ChaKing00001</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>왕</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1124,22 +1112,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>ChaMagic0001</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChaHKnight01</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChaHArcher01</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChaHMagic001</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>유닛 등급</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1276,27 +1248,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SkiKing00001</t>
-  </si>
-  <si>
-    <t>SkiKnight001</t>
-  </si>
-  <si>
-    <t>SkiArcher001</t>
-  </si>
-  <si>
-    <t>SkiMagic0001</t>
-  </si>
-  <si>
-    <t>SkiHKnight01</t>
-  </si>
-  <si>
-    <t>SkiHArcher01</t>
-  </si>
-  <si>
-    <t>SkiHMagic001</t>
-  </si>
-  <si>
     <t>스킬 코드</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1307,6 +1258,55 @@
   <si>
     <t>골드 획득량</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_K_King001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_S_Knight001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_S_Archer001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_S_Magic001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_H_Knight001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_H_Archer001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char_H_Magic001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_K_King001</t>
+  </si>
+  <si>
+    <t>Skill_S_Knight001</t>
+  </si>
+  <si>
+    <t>Skill_S_Archer001</t>
+  </si>
+  <si>
+    <t>Skill_S_Magic001</t>
+  </si>
+  <si>
+    <t>Skill_H_Knight001</t>
+  </si>
+  <si>
+    <t>Skill_H_Archer001</t>
+  </si>
+  <si>
+    <t>Skill_H_Magic001</t>
   </si>
 </sst>
 </file>
@@ -1833,7 +1833,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1852,7 +1852,7 @@
     <col min="15" max="16" width="11.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.125" customWidth="1"/>
     <col min="21" max="21" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1864,34 +1864,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>5</v>
@@ -1900,10 +1900,10 @@
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>7</v>
@@ -1912,13 +1912,13 @@
         <v>8</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -1926,10 +1926,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2" s="22">
         <v>3</v>
@@ -1944,7 +1944,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="23">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I2" s="23">
         <v>10</v>
@@ -1956,7 +1956,7 @@
         <v>5000</v>
       </c>
       <c r="L2" s="23">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="M2" s="24">
         <v>1</v>
@@ -1965,13 +1965,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P2" s="22">
         <v>10</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R2" s="22">
         <v>2</v>
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="T2" s="26" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="U2" s="22">
         <v>0</v>
@@ -1991,10 +1991,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -2009,7 +2009,7 @@
         <v>30</v>
       </c>
       <c r="H3" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" s="6">
         <v>10</v>
@@ -2036,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R3" s="5">
         <v>1.2</v>
@@ -2045,7 +2045,7 @@
         <v>2</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="U3" s="5">
         <v>10</v>
@@ -2056,10 +2056,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
@@ -2074,19 +2074,19 @@
         <v>40</v>
       </c>
       <c r="H4" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I4" s="6">
         <v>5</v>
       </c>
       <c r="J4" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="6">
         <v>80</v>
       </c>
       <c r="L4" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M4" s="7">
         <v>6</v>
@@ -2101,7 +2101,7 @@
         <v>15</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" s="5">
         <v>0.9</v>
@@ -2110,7 +2110,7 @@
         <v>1.5</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="U4" s="5">
         <v>20</v>
@@ -2121,10 +2121,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -2139,19 +2139,19 @@
         <v>40</v>
       </c>
       <c r="H5" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5" s="6">
         <v>5</v>
       </c>
       <c r="J5" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="6">
         <v>80</v>
       </c>
       <c r="L5" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M5" s="7">
         <v>3</v>
@@ -2166,7 +2166,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R5" s="5">
         <v>1</v>
@@ -2175,7 +2175,7 @@
         <v>1.5</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="U5" s="5">
         <v>30</v>
@@ -2186,10 +2186,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
@@ -2204,19 +2204,19 @@
         <v>300</v>
       </c>
       <c r="H6" s="11">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I6" s="11">
         <v>100</v>
       </c>
       <c r="J6" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K6" s="11">
         <v>1000</v>
       </c>
       <c r="L6" s="11">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="M6" s="12">
         <v>1</v>
@@ -2231,7 +2231,7 @@
         <v>10</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R6" s="10">
         <v>1.4</v>
@@ -2240,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="U6" s="10">
         <v>100</v>
@@ -2251,10 +2251,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10">
         <v>2</v>
@@ -2269,19 +2269,19 @@
         <v>400</v>
       </c>
       <c r="H7" s="11">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I7" s="11">
         <v>50</v>
       </c>
       <c r="J7" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K7" s="11">
         <v>800</v>
       </c>
       <c r="L7" s="11">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="M7" s="12">
         <v>6</v>
@@ -2296,7 +2296,7 @@
         <v>15</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R7" s="10">
         <v>1.1000000000000001</v>
@@ -2305,7 +2305,7 @@
         <v>0.75</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="U7" s="10">
         <v>200</v>
@@ -2316,10 +2316,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="10">
         <v>2</v>
@@ -2334,19 +2334,19 @@
         <v>400</v>
       </c>
       <c r="H8" s="11">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I8" s="11">
         <v>50</v>
       </c>
       <c r="J8" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K8" s="11">
         <v>800</v>
       </c>
       <c r="L8" s="11">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="M8" s="12">
         <v>3</v>
@@ -2361,7 +2361,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R8" s="10">
         <v>1.2</v>
@@ -2370,7 +2370,7 @@
         <v>0.75</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="U8" s="10">
         <v>300</v>
@@ -2403,7 +2403,7 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D3" s="27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
@@ -2412,25 +2412,25 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -2438,7 +2438,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -2453,7 +2453,7 @@
         <v>-1</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -2505,146 +2505,146 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C2" s="28" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
       <c r="F2" s="29" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="16"/>
       <c r="C3" s="16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F3" s="29"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" s="20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G10" s="19"/>
     </row>

</xml_diff>